<commit_message>
axiwrapper output with datawidth + new matrixes + new data
</commit_message>
<xml_diff>
--- a/Big_data_table.xlsx
+++ b/Big_data_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t xml:space="preserve">Total Memory</t>
   </si>
@@ -337,8 +337,8 @@
   </sheetPr>
   <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y36" activeCellId="0" sqref="Y36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AH21" activeCellId="0" sqref="AH21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2225,7 +2225,210 @@
       <c r="AI19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="0"/>
+      <c r="A20" s="1" t="n">
+        <f aca="false">(B20*C20*D20)</f>
+        <v>8192</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>2048</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1" t="n">
+        <f aca="false">V20+W20</f>
+        <v>20937</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <f aca="false">W20</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="1" t="n">
+        <f aca="false">R20</f>
+        <v>16794</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <f aca="false">X20</f>
+        <v>8</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <f aca="false">V20+W20</f>
+        <v>20937</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>16794</v>
+      </c>
+      <c r="S20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" s="1" t="n">
+        <v>3980</v>
+      </c>
+      <c r="V20" s="1" t="n">
+        <v>20937</v>
+      </c>
+      <c r="W20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z20" s="1" t="n">
+        <v>-0.472</v>
+      </c>
+      <c r="AA20" s="1" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="AB20" s="1" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="AC20" s="1" t="n">
+        <f aca="false">(1/((3.3333333333-(Z20))*10^(-3)))</f>
+        <v>262.789067977074</v>
+      </c>
+      <c r="AE20" s="1" t="n">
+        <f aca="false">AF20+AG20</f>
+        <v>3.708</v>
+      </c>
+      <c r="AF20" s="1" t="n">
+        <v>2.985</v>
+      </c>
+      <c r="AG20" s="1" t="n">
+        <v>0.723</v>
+      </c>
+      <c r="AH20" s="1" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="AI20" s="1" t="n">
+        <v>0.098</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <f aca="false">(B21*C21*D21)</f>
+        <v>8192</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>2048</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1" t="n">
+        <f aca="false">V21+W21</f>
+        <v>8769</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <f aca="false">W21</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1" t="n">
+        <f aca="false">R21</f>
+        <v>8741</v>
+      </c>
+      <c r="O21" s="1" t="n">
+        <f aca="false">X21</f>
+        <v>8</v>
+      </c>
+      <c r="Q21" s="1" t="n">
+        <f aca="false">V21+W21</f>
+        <v>8769</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <v>8741</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>1918</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <v>8769</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z21" s="0" t="n">
+        <v>-0.426</v>
+      </c>
+      <c r="AA21" s="0" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="AB21" s="0" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="AC21" s="1" t="n">
+        <f aca="false">(1/((3.3333333333-(Z21))*10^(-3)))</f>
+        <v>266.004610748945</v>
+      </c>
+      <c r="AE21" s="1" t="n">
+        <f aca="false">AF21+AG21</f>
+        <v>3.668</v>
+      </c>
+      <c r="AF21" s="0" t="n">
+        <v>2.946</v>
+      </c>
+      <c r="AG21" s="0" t="n">
+        <v>0.722</v>
+      </c>
+      <c r="AH21" s="1" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="AI21" s="1" t="n">
+        <v>0.098</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -2335,7 +2538,7 @@
         <f aca="false">(B25*C25*D25)</f>
         <v>65536</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>32</v>
       </c>
       <c r="C25" s="1" t="n">
@@ -2382,34 +2585,34 @@
         <f aca="false">V25+W25</f>
         <v>3364</v>
       </c>
-      <c r="R25" s="0" t="n">
+      <c r="R25" s="1" t="n">
         <v>2053</v>
       </c>
-      <c r="S25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" s="0" t="n">
+      <c r="S25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="U25" s="0" t="n">
+      <c r="U25" s="1" t="n">
         <v>951</v>
       </c>
-      <c r="V25" s="0" t="n">
+      <c r="V25" s="1" t="n">
         <v>3364</v>
       </c>
-      <c r="W25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X25" s="0" t="n">
+      <c r="W25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="Z25" s="0" t="n">
+      <c r="Z25" s="1" t="n">
         <v>-1.202</v>
       </c>
-      <c r="AA25" s="0" t="n">
+      <c r="AA25" s="1" t="n">
         <v>0.005</v>
       </c>
-      <c r="AB25" s="0" t="n">
+      <c r="AB25" s="1" t="n">
         <v>0.166</v>
       </c>
       <c r="AC25" s="1" t="n">
@@ -2420,10 +2623,10 @@
         <f aca="false">AF25+AG25</f>
         <v>3.883</v>
       </c>
-      <c r="AF25" s="0" t="n">
+      <c r="AF25" s="1" t="n">
         <v>3.158</v>
       </c>
-      <c r="AG25" s="0" t="n">
+      <c r="AG25" s="1" t="n">
         <v>0.725</v>
       </c>
       <c r="AH25" s="1" t="n">
@@ -2438,19 +2641,19 @@
         <f aca="false">(B26*C26*D26)</f>
         <v>32768</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>32</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>1024</v>
       </c>
-      <c r="D26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="F26" s="0" t="n">
+      <c r="D26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="F26" s="1" t="n">
         <v>14</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -2485,34 +2688,34 @@
         <f aca="false">V26+W26</f>
         <v>3295</v>
       </c>
-      <c r="R26" s="0" t="n">
+      <c r="R26" s="1" t="n">
         <v>1990</v>
       </c>
-      <c r="S26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T26" s="0" t="n">
+      <c r="S26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="U26" s="0" t="n">
+      <c r="U26" s="1" t="n">
         <v>710</v>
       </c>
-      <c r="V26" s="0" t="n">
+      <c r="V26" s="1" t="n">
         <v>3295</v>
       </c>
-      <c r="W26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X26" s="0" t="n">
+      <c r="W26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="Z26" s="0" t="n">
+      <c r="Z26" s="1" t="n">
         <v>-0.855</v>
       </c>
-      <c r="AA26" s="0" t="n">
+      <c r="AA26" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="AB26" s="0" t="n">
+      <c r="AB26" s="1" t="n">
         <v>0.166</v>
       </c>
       <c r="AC26" s="1" t="n">
@@ -2523,10 +2726,10 @@
         <f aca="false">AF26+AG26</f>
         <v>3.761</v>
       </c>
-      <c r="AF26" s="0" t="n">
+      <c r="AF26" s="1" t="n">
         <v>3.038</v>
       </c>
-      <c r="AG26" s="0" t="n">
+      <c r="AG26" s="1" t="n">
         <v>0.723</v>
       </c>
       <c r="AH26" s="1" t="n">
@@ -2541,13 +2744,13 @@
         <f aca="false">(B27*C27*D27)</f>
         <v>131072</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>8192</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="n">
@@ -2588,34 +2791,34 @@
         <f aca="false">V27+W27</f>
         <v>2100</v>
       </c>
-      <c r="R27" s="0" t="n">
+      <c r="R27" s="1" t="n">
         <v>1253</v>
       </c>
-      <c r="S27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U27" s="0" t="n">
+      <c r="S27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" s="1" t="n">
         <v>782</v>
       </c>
-      <c r="V27" s="0" t="n">
+      <c r="V27" s="1" t="n">
         <v>2100</v>
       </c>
-      <c r="W27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X27" s="0" t="n">
+      <c r="W27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="Z27" s="0" t="n">
+      <c r="Z27" s="1" t="n">
         <v>-1.765</v>
       </c>
-      <c r="AA27" s="0" t="n">
+      <c r="AA27" s="1" t="n">
         <v>0.002</v>
       </c>
-      <c r="AB27" s="0" t="n">
+      <c r="AB27" s="1" t="n">
         <v>0.166</v>
       </c>
       <c r="AC27" s="1" t="n">
@@ -2626,10 +2829,10 @@
         <f aca="false">AF27+AG27</f>
         <v>3.833</v>
       </c>
-      <c r="AF27" s="0" t="n">
+      <c r="AF27" s="1" t="n">
         <v>3.108</v>
       </c>
-      <c r="AG27" s="0" t="n">
+      <c r="AG27" s="1" t="n">
         <v>0.725</v>
       </c>
       <c r="AH27" s="1" t="n">
@@ -2644,13 +2847,13 @@
         <f aca="false">(B28*C28*D28)</f>
         <v>65536</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="n">
@@ -2691,34 +2894,34 @@
         <f aca="false">V28+W28</f>
         <v>1790</v>
       </c>
-      <c r="R28" s="0" t="n">
+      <c r="R28" s="1" t="n">
         <v>1222</v>
       </c>
-      <c r="S28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U28" s="0" t="n">
+      <c r="S28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" s="1" t="n">
         <v>571</v>
       </c>
-      <c r="V28" s="0" t="n">
+      <c r="V28" s="1" t="n">
         <v>1790</v>
       </c>
-      <c r="W28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X28" s="0" t="n">
+      <c r="W28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="Z28" s="0" t="n">
+      <c r="Z28" s="1" t="n">
         <v>-0.966</v>
       </c>
-      <c r="AA28" s="0" t="n">
+      <c r="AA28" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="AB28" s="0" t="n">
+      <c r="AB28" s="1" t="n">
         <v>0.166</v>
       </c>
       <c r="AC28" s="1" t="n">
@@ -2729,10 +2932,10 @@
         <f aca="false">AF28+AG28</f>
         <v>3.813</v>
       </c>
-      <c r="AF28" s="0" t="n">
+      <c r="AF28" s="1" t="n">
         <v>3.089</v>
       </c>
-      <c r="AG28" s="0" t="n">
+      <c r="AG28" s="1" t="n">
         <v>0.724</v>
       </c>
       <c r="AH28" s="1" t="n">
@@ -2747,13 +2950,13 @@
         <f aca="false">(B29*C29*D29)</f>
         <v>32768</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="1" t="n">
@@ -2794,34 +2997,34 @@
         <f aca="false">V29+W29</f>
         <v>1670</v>
       </c>
-      <c r="R29" s="0" t="n">
+      <c r="R29" s="1" t="n">
         <v>1190</v>
       </c>
-      <c r="S29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U29" s="0" t="n">
+      <c r="S29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" s="1" t="n">
         <v>479</v>
       </c>
-      <c r="V29" s="0" t="n">
+      <c r="V29" s="1" t="n">
         <v>1670</v>
       </c>
-      <c r="W29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X29" s="0" t="n">
+      <c r="W29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="Z29" s="0" t="n">
+      <c r="Z29" s="1" t="n">
         <v>-0.589</v>
       </c>
-      <c r="AA29" s="0" t="n">
+      <c r="AA29" s="1" t="n">
         <v>0.014</v>
       </c>
-      <c r="AB29" s="0" t="n">
+      <c r="AB29" s="1" t="n">
         <v>0.166</v>
       </c>
       <c r="AC29" s="1" t="n">
@@ -2832,10 +3035,10 @@
         <f aca="false">AF29+AG29</f>
         <v>3.711</v>
       </c>
-      <c r="AF29" s="0" t="n">
+      <c r="AF29" s="1" t="n">
         <v>2.988</v>
       </c>
-      <c r="AG29" s="0" t="n">
+      <c r="AG29" s="1" t="n">
         <v>0.723</v>
       </c>
       <c r="AH29" s="1" t="n">
@@ -2850,19 +3053,19 @@
         <f aca="false">(B30*C30*D30)</f>
         <v>65536</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E30" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="F30" s="0" t="n">
+      <c r="E30" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="F30" s="1" t="n">
         <v>14</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -2897,34 +3100,34 @@
         <f aca="false">V30+W30</f>
         <v>3160</v>
       </c>
-      <c r="R30" s="0" t="n">
+      <c r="R30" s="1" t="n">
         <v>1685</v>
       </c>
-      <c r="S30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U30" s="0" t="n">
+      <c r="S30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" s="1" t="n">
         <v>786</v>
       </c>
-      <c r="V30" s="0" t="n">
+      <c r="V30" s="1" t="n">
         <v>3160</v>
       </c>
-      <c r="W30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X30" s="0" t="n">
+      <c r="W30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="Z30" s="0" t="n">
+      <c r="Z30" s="1" t="n">
         <v>-1.367</v>
       </c>
-      <c r="AA30" s="0" t="n">
+      <c r="AA30" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="AB30" s="0" t="n">
+      <c r="AB30" s="1" t="n">
         <v>0.166</v>
       </c>
       <c r="AC30" s="1" t="n">
@@ -2935,10 +3138,10 @@
         <f aca="false">AF30+AG30</f>
         <v>3.83</v>
       </c>
-      <c r="AF30" s="0" t="n">
+      <c r="AF30" s="1" t="n">
         <v>3.106</v>
       </c>
-      <c r="AG30" s="0" t="n">
+      <c r="AG30" s="1" t="n">
         <v>0.724</v>
       </c>
       <c r="AH30" s="1" t="n">
@@ -2953,13 +3156,13 @@
         <f aca="false">(B31*C31*D31)</f>
         <v>131072</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E31" s="1" t="n">
@@ -3000,34 +3203,34 @@
         <f aca="false">V31+W31</f>
         <v>5576</v>
       </c>
-      <c r="R31" s="0" t="n">
+      <c r="R31" s="1" t="n">
         <v>2680</v>
       </c>
-      <c r="S31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U31" s="0" t="n">
+      <c r="S31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" s="1" t="n">
         <v>1425</v>
       </c>
-      <c r="V31" s="0" t="n">
+      <c r="V31" s="1" t="n">
         <v>5576</v>
       </c>
-      <c r="W31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X31" s="0" t="n">
+      <c r="W31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="Z31" s="0" t="n">
+      <c r="Z31" s="1" t="n">
         <v>-2.08</v>
       </c>
-      <c r="AA31" s="0" t="n">
+      <c r="AA31" s="1" t="n">
         <v>0.019</v>
       </c>
-      <c r="AB31" s="0" t="n">
+      <c r="AB31" s="1" t="n">
         <v>0.166</v>
       </c>
       <c r="AC31" s="1" t="n">
@@ -3038,10 +3241,10 @@
         <f aca="false">AF31+AG31</f>
         <v>4.032</v>
       </c>
-      <c r="AF31" s="0" t="n">
+      <c r="AF31" s="1" t="n">
         <v>3.306</v>
       </c>
-      <c r="AG31" s="0" t="n">
+      <c r="AG31" s="1" t="n">
         <v>0.726</v>
       </c>
       <c r="AH31" s="1" t="n">
@@ -3056,13 +3259,13 @@
         <f aca="false">(B32*C32*D32)</f>
         <v>32768</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>1024</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E32" s="1" t="n">
@@ -3103,34 +3306,34 @@
         <f aca="false">V32+W32</f>
         <v>3060</v>
       </c>
-      <c r="R32" s="0" t="n">
+      <c r="R32" s="1" t="n">
         <v>1653</v>
       </c>
-      <c r="S32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U32" s="0" t="n">
+      <c r="S32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" s="1" t="n">
         <v>676</v>
       </c>
-      <c r="V32" s="0" t="n">
+      <c r="V32" s="1" t="n">
         <v>3060</v>
       </c>
-      <c r="W32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X32" s="0" t="n">
+      <c r="W32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="Z32" s="0" t="n">
+      <c r="Z32" s="1" t="n">
         <v>-0.903</v>
       </c>
-      <c r="AA32" s="0" t="n">
+      <c r="AA32" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="AB32" s="0" t="n">
+      <c r="AB32" s="1" t="n">
         <v>0.166</v>
       </c>
       <c r="AC32" s="1" t="n">
@@ -3141,10 +3344,10 @@
         <f aca="false">AF32+AG32</f>
         <v>3.751</v>
       </c>
-      <c r="AF32" s="0" t="n">
+      <c r="AF32" s="1" t="n">
         <v>3.028</v>
       </c>
-      <c r="AG32" s="0" t="n">
+      <c r="AG32" s="1" t="n">
         <v>0.723</v>
       </c>
       <c r="AH32" s="1" t="n">
@@ -3157,7 +3360,104 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <f aca="false">(B33*C33*D33)</f>
-        <v>0</v>
+        <v>32768</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <f aca="false">V33+W33</f>
+        <v>5365</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <f aca="false">W33</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="n">
+        <f aca="false">R33</f>
+        <v>2618</v>
+      </c>
+      <c r="O33" s="1" t="n">
+        <f aca="false">X33</f>
+        <v>32</v>
+      </c>
+      <c r="Q33" s="1" t="n">
+        <f aca="false">V33+W33</f>
+        <v>5365</v>
+      </c>
+      <c r="R33" s="1" t="n">
+        <v>2618</v>
+      </c>
+      <c r="S33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="U33" s="1" t="n">
+        <v>1010</v>
+      </c>
+      <c r="V33" s="1" t="n">
+        <v>5365</v>
+      </c>
+      <c r="W33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="Z33" s="1" t="n">
+        <v>-1.1</v>
+      </c>
+      <c r="AA33" s="1" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="AB33" s="1" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="AC33" s="1" t="n">
+        <f aca="false">(1/((3.3333333333-(Z33))*10^(-3)))</f>
+        <v>225.563909776132</v>
+      </c>
+      <c r="AE33" s="1" t="n">
+        <f aca="false">AF33+AG33</f>
+        <v>3.94</v>
+      </c>
+      <c r="AF33" s="1" t="n">
+        <v>3.215</v>
+      </c>
+      <c r="AG33" s="1" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="AH33" s="1" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="AI33" s="1" t="n">
+        <v>0.098</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3191,10 +3491,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="1" t="n">
         <v>1.1</v>
       </c>
       <c r="C48" s="1" t="s">

</xml_diff>